<commit_message>
ICDC multi test cases updated for OSA03
</commit_message>
<xml_diff>
--- a/InputFiles/ICDC/TC36_Canine_Study_OSA03_SamplePathology-OsteoblasticOsteosarcoma.xlsx
+++ b/InputFiles/ICDC/TC36_Canine_Study_OSA03_SamplePathology-OsteoblasticOsteosarcoma.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\podagatlapalll2\ICDC Automation\ICDCPrasanna\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epishinavv\git\Commons_Automation\InputFiles\ICDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8316B53B-F3B8-4C5A-8603-5A1CFDFB536B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B0B4EC-326E-49D2-91CF-C4DDB402F093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -573,7 +573,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="44" zoomScaleNormal="44" zoomScalePageLayoutView="56" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>